<commit_message>
Edit plots to include CPU baseline for relative
</commit_message>
<xml_diff>
--- a/writeup/rawdata.xlsx
+++ b/writeup/rawdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z799j\Documents\UPENN\CIS5650\Project2-Stream-Compaction\writeup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683758BB-31AE-44DC-9C47-22373393B33D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEBF78A-DBAE-46B4-8557-D6E5D2419AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB196A8B-504A-45AD-8296-ECCD6F7C157D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FB196A8B-504A-45AD-8296-ECCD6F7C157D}"/>
   </bookViews>
   <sheets>
     <sheet name="ScanCompactSort" sheetId="1" r:id="rId1"/>
@@ -3017,8 +3017,63 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CPU Compact without Scan</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ScanCompactSort!$I$53:$O$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E15F-429D-BB4B-EEBF8AFDC116}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$48</c:f>
@@ -3111,7 +3166,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$49</c:f>
@@ -5409,8 +5464,57 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>CPU Sort</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ScanCompactSort!$E$53:$I$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F3D3-4532-B726-7F50E60F9ED1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$50</c:f>
@@ -5491,7 +5595,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$51</c:f>
@@ -8832,8 +8936,77 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ScanCompactSort!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU Scan Po2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ScanCompactSort!$B$53:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-07ED-49A3-8C7E-1D2ECE30F109}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$42</c:f>
@@ -8938,7 +9111,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$44</c:f>
@@ -9043,7 +9216,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$46</c:f>
@@ -9589,8 +9762,74 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ScanCompactSort!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU Scan Po2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ScanCompactSort!$J$53:$Q$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD05-443A-8A4D-72D0816560BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$42</c:f>
@@ -9689,7 +9928,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$44</c:f>
@@ -9788,7 +10027,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$46</c:f>
@@ -10328,8 +10567,77 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ScanCompactSort!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU Scan NPo2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ScanCompactSort!$B$53:$J$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0A4C-48A9-8E10-CB58CF04BB5F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$43</c:f>
@@ -10434,7 +10742,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$45</c:f>
@@ -10539,7 +10847,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$47</c:f>
@@ -11085,8 +11393,74 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ScanCompactSort!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPU Scan NPo2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>ScanCompactSort!$J$53:$Q$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8114-496D-AC94-A41CCD0FD459}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$43</c:f>
@@ -11185,7 +11559,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$45</c:f>
@@ -11284,7 +11658,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>ScanCompactSort!$A$47</c:f>
@@ -21286,18 +21660,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244C1008-F460-4F46-99E2-B5AE772836E8}">
-  <dimension ref="A1:DH51"/>
+  <dimension ref="A1:DH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T83" sqref="T83"/>
+    <sheetView tabSelected="1" topLeftCell="K71" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AI96" sqref="AI96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -21395,7 +21769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -21704,7 +22078,7 @@
         <v>9.2000000000000014E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -22009,11 +22383,11 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="DH3">
-        <f t="shared" ref="DH3:DH18" si="15">AVERAGE(DC3:DG3)</f>
+        <f t="shared" ref="DH3:DH17" si="15">AVERAGE(DC3:DG3)</f>
         <v>5.8E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -22322,7 +22696,7 @@
         <v>0.13168640000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -22631,7 +23005,7 @@
         <v>2.1503999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -22940,7 +23314,7 @@
         <v>0.16936959999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -23249,7 +23623,7 @@
         <v>4.9382400000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -23558,7 +23932,7 @@
         <v>0.2118208</v>
       </c>
     </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -23867,7 +24241,7 @@
         <v>3.5097599999999993E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -24176,7 +24550,7 @@
         <v>1.8799999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -24485,7 +24859,7 @@
         <v>1.8599999999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -24794,7 +25168,7 @@
         <v>4.4600000000000004E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -25103,7 +25477,7 @@
         <v>0.18124800000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -25412,7 +25786,7 @@
         <v>9.2159999999999992E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -25721,7 +26095,7 @@
         <v>2.8420000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -26030,7 +26404,7 @@
         <v>2.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -26339,7 +26713,7 @@
         <v>0.98551800000000012</v>
       </c>
     </row>
-    <row r="18" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -26648,12 +27022,12 @@
         <v>0.96071639999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -26706,7 +27080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -26759,7 +27133,7 @@
         <v>17.585039999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -26812,7 +27186,7 @@
         <v>17.746339999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -26865,7 +27239,7 @@
         <v>14.614339999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -26918,7 +27292,7 @@
         <v>14.443520000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -26971,7 +27345,7 @@
         <v>6.1558779999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -27024,7 +27398,7 @@
         <v>5.6422400000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -27077,7 +27451,7 @@
         <v>1.0426123999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -27130,7 +27504,7 @@
         <v>0.63673599999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -27183,7 +27557,7 @@
         <v>48.963760000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:112" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:112" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -27236,7 +27610,7 @@
         <v>47.86786</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -27289,7 +27663,7 @@
         <v>128.68119999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -27342,7 +27716,7 @@
         <v>17.472100000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -27395,7 +27769,7 @@
         <v>10.314960000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -27448,7 +27822,7 @@
         <v>1332.674</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -27501,7 +27875,7 @@
         <v>1332.088</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -27554,7 +27928,7 @@
         <v>389.15699999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -27607,12 +27981,12 @@
         <v>388.61419999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -27681,7 +28055,7 @@
         <v>0.831066633911552</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -27690,7 +28064,7 @@
         <v>37.075862068965513</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C43:Q43" si="17">C26/C24</f>
+        <f t="shared" ref="C43:P43" si="17">C26/C24</f>
         <v>69.459199999999981</v>
       </c>
       <c r="D43">
@@ -27750,7 +28124,7 @@
         <v>0.81388725787965321</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -27759,7 +28133,7 @@
         <v>184.09739130434775</v>
       </c>
       <c r="C44">
-        <f t="shared" ref="C44:Q44" si="18">C27/C23</f>
+        <f t="shared" ref="C44:P44" si="18">C27/C23</f>
         <v>100.352</v>
       </c>
       <c r="D44">
@@ -27819,7 +28193,7 @@
         <v>0.35006334930145167</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -27828,7 +28202,7 @@
         <v>85.142068965517254</v>
       </c>
       <c r="C45">
-        <f t="shared" ref="C45:Q45" si="19">C28/C24</f>
+        <f t="shared" ref="C45:P45" si="19">C28/C24</f>
         <v>53.657599999999995</v>
       </c>
       <c r="D45">
@@ -27888,7 +28262,7 @@
         <v>0.31793823402459331</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -27957,7 +28331,7 @@
         <v>5.928973718569875E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -27966,7 +28340,7 @@
         <v>60.513103448275849</v>
       </c>
       <c r="C47">
-        <f t="shared" ref="C47:Q47" si="21">C30/C24</f>
+        <f t="shared" ref="C47:P47" si="21">C30/C24</f>
         <v>33.63839999999999</v>
       </c>
       <c r="D47">
@@ -28026,7 +28400,7 @@
         <v>3.5879849028024942E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -28095,7 +28469,7 @@
         <v>0.35683738340356214</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -28104,7 +28478,7 @@
         <v>49.548387096774192</v>
       </c>
       <c r="C49">
-        <f t="shared" ref="C49:Q49" si="23">C35/C32</f>
+        <f t="shared" ref="C49:P49" si="23">C35/C32</f>
         <v>26.236540540540535</v>
       </c>
       <c r="D49">
@@ -28164,7 +28538,7 @@
         <v>0.21548822111537891</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -28233,7 +28607,7 @@
         <v>0.29201215000817904</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -28242,7 +28616,7 @@
         <v>32.677428571428571</v>
       </c>
       <c r="C51">
-        <f t="shared" ref="C51:Q51" si="25">C39/C37</f>
+        <f t="shared" ref="C51:P51" si="25">C39/C37</f>
         <v>15.724325371207231</v>
       </c>
       <c r="D51">
@@ -28300,6 +28674,56 @@
       <c r="Q51">
         <f>Q39/Q37</f>
         <v>0.29173312874224527</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53">
+        <v>1</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
+      </c>
+      <c r="P53">
+        <v>1</v>
+      </c>
+      <c r="Q53">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Readme added with figures and explanations
</commit_message>
<xml_diff>
--- a/writeup/rawdata.xlsx
+++ b/writeup/rawdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z799j\Documents\UPENN\CIS5650\Project2-Stream-Compaction\writeup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEBF78A-DBAE-46B4-8557-D6E5D2419AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5525E04-46EA-49B7-A8EE-E52F265694A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{FB196A8B-504A-45AD-8296-ECCD6F7C157D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB196A8B-504A-45AD-8296-ECCD6F7C157D}"/>
   </bookViews>
   <sheets>
     <sheet name="ScanCompactSort" sheetId="1" r:id="rId1"/>
@@ -3467,7 +3467,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (ms)</a:t>
+                  <a:t>Performance Relative to CPU</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5884,7 +5884,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (ms)</a:t>
+                  <a:t>Performance Relative to CPU</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -9529,7 +9529,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (ms)</a:t>
+                  <a:t>Performance Relative to CPU</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -10334,7 +10334,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (ms)</a:t>
+                  <a:t>Performance Relative to CPU</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11160,7 +11160,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (ms)</a:t>
+                  <a:t>Performance Relative to CPU</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -11965,7 +11965,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Time (ms)</a:t>
+                  <a:t>Performance Relative to CPU</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -21117,13 +21117,13 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>136072</xdr:colOff>
       <xdr:row>61</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>340580</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>17691</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>117724</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -21662,16 +21662,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244C1008-F460-4F46-99E2-B5AE772836E8}">
   <dimension ref="A1:DH53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K71" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AI96" sqref="AI96"/>
+    <sheetView tabSelected="1" topLeftCell="G73" zoomScale="89" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE85" sqref="AE85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:112" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -21769,7 +21769,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -22078,7 +22078,7 @@
         <v>9.2000000000000014E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -22387,7 +22387,7 @@
         <v>5.8E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -22696,7 +22696,7 @@
         <v>0.13168640000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -23005,7 +23005,7 @@
         <v>2.1503999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -23314,7 +23314,7 @@
         <v>0.16936959999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -23623,7 +23623,7 @@
         <v>4.9382400000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -23932,7 +23932,7 @@
         <v>0.2118208</v>
       </c>
     </row>
-    <row r="9" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -24241,7 +24241,7 @@
         <v>3.5097599999999993E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -24550,7 +24550,7 @@
         <v>1.8799999999999997E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -24859,7 +24859,7 @@
         <v>1.8599999999999999E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -25168,7 +25168,7 @@
         <v>4.4600000000000004E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -25477,7 +25477,7 @@
         <v>0.18124800000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -25786,7 +25786,7 @@
         <v>9.2159999999999992E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -26095,7 +26095,7 @@
         <v>2.8420000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -26404,7 +26404,7 @@
         <v>2.9399999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -26713,7 +26713,7 @@
         <v>0.98551800000000012</v>
       </c>
     </row>
-    <row r="18" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -27022,12 +27022,12 @@
         <v>0.96071639999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -27080,7 +27080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -27133,7 +27133,7 @@
         <v>17.585039999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -27186,7 +27186,7 @@
         <v>17.746339999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -27239,7 +27239,7 @@
         <v>14.614339999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -27292,7 +27292,7 @@
         <v>14.443520000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -27345,7 +27345,7 @@
         <v>6.1558779999999995</v>
       </c>
     </row>
-    <row r="28" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -27398,7 +27398,7 @@
         <v>5.6422400000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -27451,7 +27451,7 @@
         <v>1.0426123999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -27504,7 +27504,7 @@
         <v>0.63673599999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -27557,7 +27557,7 @@
         <v>48.963760000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:112" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:112" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -27610,7 +27610,7 @@
         <v>47.86786</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -27663,7 +27663,7 @@
         <v>128.68119999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>29</v>
       </c>
@@ -27716,7 +27716,7 @@
         <v>17.472100000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -27769,7 +27769,7 @@
         <v>10.314960000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -27822,7 +27822,7 @@
         <v>1332.674</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -27875,7 +27875,7 @@
         <v>1332.088</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -27928,7 +27928,7 @@
         <v>389.15699999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>34</v>
       </c>
@@ -27981,12 +27981,12 @@
         <v>388.61419999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -28055,7 +28055,7 @@
         <v>0.831066633911552</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -28124,7 +28124,7 @@
         <v>0.81388725787965321</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -28193,7 +28193,7 @@
         <v>0.35006334930145167</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -28262,7 +28262,7 @@
         <v>0.31793823402459331</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -28331,7 +28331,7 @@
         <v>5.928973718569875E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -28400,7 +28400,7 @@
         <v>3.5879849028024942E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>29</v>
       </c>
@@ -28469,7 +28469,7 @@
         <v>0.35683738340356214</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -28538,7 +28538,7 @@
         <v>0.21548822111537891</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>33</v>
       </c>
@@ -28607,7 +28607,7 @@
         <v>0.29201215000817904</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>34</v>
       </c>
@@ -28676,7 +28676,7 @@
         <v>0.29173312874224527</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B53">
         <v>1</v>
       </c>

</xml_diff>